<commit_message>
Routage done, mais revoir schématique
</commit_message>
<xml_diff>
--- a/Documentation/Liste des Pins.xlsx
+++ b/Documentation/Liste des Pins.xlsx
@@ -725,697 +725,699 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E45"/>
+  <dimension ref="B1:F46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="D28" sqref="D28"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H4" sqref="H4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="3.28515625" style="2" customWidth="1"/>
-    <col min="2" max="2" width="4.28515625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="3.5703125" style="1" customWidth="1"/>
-    <col min="4" max="4" width="38.5703125" style="1" customWidth="1"/>
-    <col min="5" max="5" width="53.5703125" style="1" customWidth="1"/>
+    <col min="1" max="1" width="2.7109375" customWidth="1"/>
+    <col min="2" max="2" width="3.28515625" style="2" customWidth="1"/>
+    <col min="3" max="3" width="4.28515625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="3.5703125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="38.5703125" style="1" customWidth="1"/>
+    <col min="6" max="6" width="53.5703125" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="4" customFormat="1" ht="15.75" thickBot="1">
-      <c r="A1" s="3" t="s">
+    <row r="1" spans="2:6" ht="15.75" thickBot="1"/>
+    <row r="2" spans="2:6" s="4" customFormat="1" ht="15.75" thickBot="1">
+      <c r="B2" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="9" t="s">
+      <c r="C2" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="C1" s="16" t="s">
+      <c r="D2" s="16" t="s">
         <v>4</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="E2" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="9" t="s">
+      <c r="F2" s="9" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:5">
-      <c r="A2" s="13">
+    <row r="3" spans="2:6">
+      <c r="B3" s="13">
         <v>1</v>
       </c>
-      <c r="B2" s="10">
-        <v>9</v>
-      </c>
-      <c r="C2" s="17" t="s">
-        <v>5</v>
-      </c>
-      <c r="D2" s="6" t="s">
+      <c r="C3" s="10">
+        <v>9</v>
+      </c>
+      <c r="D3" s="17" t="s">
+        <v>5</v>
+      </c>
+      <c r="E3" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="E2" s="10"/>
-    </row>
-    <row r="3" spans="1:5">
-      <c r="A3" s="14">
+      <c r="F3" s="10"/>
+    </row>
+    <row r="4" spans="2:6">
+      <c r="B4" s="14">
         <v>2</v>
       </c>
-      <c r="B3" s="11">
+      <c r="C4" s="11">
         <v>22</v>
       </c>
-      <c r="C3" s="18" t="s">
-        <v>5</v>
-      </c>
-      <c r="D3" s="7" t="s">
+      <c r="D4" s="18" t="s">
+        <v>5</v>
+      </c>
+      <c r="E4" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="E3" s="11"/>
-    </row>
-    <row r="4" spans="1:5">
-      <c r="A4" s="14">
+      <c r="F4" s="11"/>
+    </row>
+    <row r="5" spans="2:6">
+      <c r="B5" s="14">
         <v>3</v>
       </c>
-      <c r="B4" s="11">
+      <c r="C5" s="11">
         <v>23</v>
       </c>
-      <c r="C4" s="18" t="s">
-        <v>5</v>
-      </c>
-      <c r="D4" s="7" t="s">
+      <c r="D5" s="18" t="s">
+        <v>5</v>
+      </c>
+      <c r="E5" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="E4" s="11"/>
-    </row>
-    <row r="5" spans="1:5">
-      <c r="A5" s="14">
+      <c r="F5" s="11"/>
+    </row>
+    <row r="6" spans="2:6">
+      <c r="B6" s="14">
         <v>4</v>
       </c>
-      <c r="B5" s="11">
+      <c r="C6" s="11">
         <v>24</v>
       </c>
-      <c r="C5" s="18" t="s">
-        <v>5</v>
-      </c>
-      <c r="D5" s="7" t="s">
+      <c r="D6" s="18" t="s">
+        <v>5</v>
+      </c>
+      <c r="E6" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="E5" s="11"/>
-    </row>
-    <row r="6" spans="1:5">
-      <c r="A6" s="14">
-        <v>5</v>
-      </c>
-      <c r="B6" s="11">
+      <c r="F6" s="11"/>
+    </row>
+    <row r="7" spans="2:6">
+      <c r="B7" s="14">
+        <v>5</v>
+      </c>
+      <c r="C7" s="11">
         <v>25</v>
       </c>
-      <c r="C6" s="18" t="s">
-        <v>5</v>
-      </c>
-      <c r="D6" s="7" t="s">
+      <c r="D7" s="18" t="s">
+        <v>5</v>
+      </c>
+      <c r="E7" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="E6" s="11"/>
-    </row>
-    <row r="7" spans="1:5">
-      <c r="A7" s="14">
-        <v>6</v>
-      </c>
-      <c r="B7" s="11" t="s">
-        <v>6</v>
-      </c>
-      <c r="C7" s="18" t="s">
-        <v>9</v>
-      </c>
-      <c r="D7" s="7" t="s">
+      <c r="F7" s="11"/>
+    </row>
+    <row r="8" spans="2:6">
+      <c r="B8" s="14">
+        <v>6</v>
+      </c>
+      <c r="C8" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="D8" s="18" t="s">
+        <v>9</v>
+      </c>
+      <c r="E8" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="E7" s="11"/>
-    </row>
-    <row r="8" spans="1:5">
-      <c r="A8" s="14">
+      <c r="F8" s="11"/>
+    </row>
+    <row r="9" spans="2:6">
+      <c r="B9" s="14">
         <v>7</v>
       </c>
-      <c r="B8" s="11" t="s">
-        <v>6</v>
-      </c>
-      <c r="C8" s="18" t="s">
-        <v>9</v>
-      </c>
-      <c r="D8" s="7" t="s">
+      <c r="C9" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="D9" s="18" t="s">
+        <v>9</v>
+      </c>
+      <c r="E9" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="E8" s="11"/>
-    </row>
-    <row r="9" spans="1:5" s="25" customFormat="1" ht="30">
-      <c r="A9" s="21">
+      <c r="F9" s="11"/>
+    </row>
+    <row r="10" spans="2:6" s="25" customFormat="1" ht="30">
+      <c r="B10" s="21">
         <v>8</v>
       </c>
-      <c r="B9" s="22">
+      <c r="C10" s="22">
         <v>10</v>
       </c>
-      <c r="C9" s="23" t="s">
-        <v>5</v>
-      </c>
-      <c r="D9" s="24" t="s">
+      <c r="D10" s="23" t="s">
+        <v>5</v>
+      </c>
+      <c r="E10" s="24" t="s">
         <v>42</v>
       </c>
-      <c r="E9" s="22"/>
-    </row>
-    <row r="10" spans="1:5">
-      <c r="A10" s="14">
-        <v>9</v>
-      </c>
-      <c r="B10" s="11">
+      <c r="F10" s="22"/>
+    </row>
+    <row r="11" spans="2:6">
+      <c r="B11" s="14">
+        <v>9</v>
+      </c>
+      <c r="C11" s="11">
         <v>11</v>
       </c>
-      <c r="C10" s="18" t="s">
-        <v>5</v>
-      </c>
-      <c r="D10" s="7" t="s">
+      <c r="D11" s="18" t="s">
+        <v>5</v>
+      </c>
+      <c r="E11" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="E10" s="11"/>
-    </row>
-    <row r="11" spans="1:5">
-      <c r="A11" s="14">
+      <c r="F11" s="11"/>
+    </row>
+    <row r="12" spans="2:6">
+      <c r="B12" s="14">
         <v>10</v>
       </c>
-      <c r="B11" s="11">
+      <c r="C12" s="11">
         <v>12</v>
       </c>
-      <c r="C11" s="18" t="s">
-        <v>9</v>
-      </c>
-      <c r="D11" s="7" t="s">
+      <c r="D12" s="18" t="s">
+        <v>9</v>
+      </c>
+      <c r="E12" s="7" t="s">
         <v>43</v>
       </c>
-      <c r="E11" s="11"/>
-    </row>
-    <row r="12" spans="1:5" ht="15.75" thickBot="1">
-      <c r="A12" s="15">
+      <c r="F12" s="11"/>
+    </row>
+    <row r="13" spans="2:6" ht="15.75" thickBot="1">
+      <c r="B13" s="15">
         <v>11</v>
       </c>
-      <c r="B12" s="12">
+      <c r="C13" s="12">
         <v>13</v>
       </c>
-      <c r="C12" s="19" t="s">
-        <v>9</v>
-      </c>
-      <c r="D12" s="8" t="s">
+      <c r="D13" s="19" t="s">
+        <v>9</v>
+      </c>
+      <c r="E13" s="8" t="s">
         <v>44</v>
       </c>
-      <c r="E12" s="12"/>
-    </row>
-    <row r="13" spans="1:5">
-      <c r="A13" s="13">
+      <c r="F13" s="12"/>
+    </row>
+    <row r="14" spans="2:6">
+      <c r="B14" s="13">
         <v>12</v>
       </c>
-      <c r="B13" s="10" t="s">
-        <v>6</v>
-      </c>
-      <c r="C13" s="17" t="s">
-        <v>5</v>
-      </c>
-      <c r="D13" s="6" t="s">
+      <c r="C14" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="D14" s="17" t="s">
+        <v>5</v>
+      </c>
+      <c r="E14" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="E13" s="10"/>
-    </row>
-    <row r="14" spans="1:5">
-      <c r="A14" s="14">
+      <c r="F14" s="10"/>
+    </row>
+    <row r="15" spans="2:6">
+      <c r="B15" s="14">
         <v>13</v>
       </c>
-      <c r="B14" s="11" t="s">
-        <v>6</v>
-      </c>
-      <c r="C14" s="18" t="s">
-        <v>5</v>
-      </c>
-      <c r="D14" s="7" t="s">
+      <c r="C15" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="D15" s="18" t="s">
+        <v>5</v>
+      </c>
+      <c r="E15" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="E14" s="11"/>
-    </row>
-    <row r="15" spans="1:5" ht="30">
-      <c r="A15" s="14">
+      <c r="F15" s="11"/>
+    </row>
+    <row r="16" spans="2:6" ht="30">
+      <c r="B16" s="14">
         <v>14</v>
       </c>
-      <c r="B15" s="11">
+      <c r="C16" s="11">
         <v>14</v>
       </c>
-      <c r="C15" s="18" t="s">
-        <v>9</v>
-      </c>
-      <c r="D15" s="20" t="s">
+      <c r="D16" s="18" t="s">
+        <v>9</v>
+      </c>
+      <c r="E16" s="20" t="s">
         <v>45</v>
       </c>
-      <c r="E15" s="11"/>
-    </row>
-    <row r="16" spans="1:5">
-      <c r="A16" s="14">
+      <c r="F16" s="11"/>
+    </row>
+    <row r="17" spans="2:6">
+      <c r="B17" s="14">
         <v>15</v>
       </c>
-      <c r="B16" s="11">
+      <c r="C17" s="11">
         <v>15</v>
       </c>
-      <c r="C16" s="18" t="s">
-        <v>9</v>
-      </c>
-      <c r="D16" s="7" t="s">
+      <c r="D17" s="18" t="s">
+        <v>9</v>
+      </c>
+      <c r="E17" s="7" t="s">
         <v>46</v>
       </c>
-      <c r="E16" s="11"/>
-    </row>
-    <row r="17" spans="1:5">
-      <c r="A17" s="14">
+      <c r="F17" s="11"/>
+    </row>
+    <row r="18" spans="2:6">
+      <c r="B18" s="14">
         <v>16</v>
       </c>
-      <c r="B17" s="11" t="s">
-        <v>6</v>
-      </c>
-      <c r="C17" s="18" t="s">
-        <v>9</v>
-      </c>
-      <c r="D17" s="7" t="s">
+      <c r="C18" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="D18" s="18" t="s">
+        <v>9</v>
+      </c>
+      <c r="E18" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="E17" s="11"/>
-    </row>
-    <row r="18" spans="1:5">
-      <c r="A18" s="14">
+      <c r="F18" s="11"/>
+    </row>
+    <row r="19" spans="2:6">
+      <c r="B19" s="14">
         <v>17</v>
       </c>
-      <c r="B18" s="11" t="s">
-        <v>6</v>
-      </c>
-      <c r="C18" s="18" t="s">
-        <v>9</v>
-      </c>
-      <c r="D18" s="7" t="s">
+      <c r="C19" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="D19" s="18" t="s">
+        <v>9</v>
+      </c>
+      <c r="E19" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="E18" s="11"/>
-    </row>
-    <row r="19" spans="1:5">
-      <c r="A19" s="14">
+      <c r="F19" s="11"/>
+    </row>
+    <row r="20" spans="2:6">
+      <c r="B20" s="14">
         <v>18</v>
       </c>
-      <c r="B19" s="11" t="s">
-        <v>6</v>
-      </c>
-      <c r="C19" s="18" t="s">
-        <v>5</v>
-      </c>
-      <c r="D19" s="7" t="s">
+      <c r="C20" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="D20" s="18" t="s">
+        <v>5</v>
+      </c>
+      <c r="E20" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="E19" s="11"/>
-    </row>
-    <row r="20" spans="1:5">
-      <c r="A20" s="14">
+      <c r="F20" s="11"/>
+    </row>
+    <row r="21" spans="2:6">
+      <c r="B21" s="14">
         <v>19</v>
       </c>
-      <c r="B20" s="11" t="s">
-        <v>6</v>
-      </c>
-      <c r="C20" s="18" t="s">
-        <v>9</v>
-      </c>
-      <c r="D20" s="7" t="s">
+      <c r="C21" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="D21" s="18" t="s">
+        <v>9</v>
+      </c>
+      <c r="E21" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="E20" s="11"/>
-    </row>
-    <row r="21" spans="1:5">
-      <c r="A21" s="14">
+      <c r="F21" s="11"/>
+    </row>
+    <row r="22" spans="2:6">
+      <c r="B22" s="14">
         <v>20</v>
       </c>
-      <c r="B21" s="11" t="s">
-        <v>6</v>
-      </c>
-      <c r="C21" s="18" t="s">
-        <v>9</v>
-      </c>
-      <c r="D21" s="7" t="s">
+      <c r="C22" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="D22" s="18" t="s">
+        <v>9</v>
+      </c>
+      <c r="E22" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="E21" s="11"/>
-    </row>
-    <row r="22" spans="1:5">
-      <c r="A22" s="14">
+      <c r="F22" s="11"/>
+    </row>
+    <row r="23" spans="2:6">
+      <c r="B23" s="14">
         <v>21</v>
       </c>
-      <c r="B22" s="11">
+      <c r="C23" s="11">
         <v>0</v>
       </c>
-      <c r="C22" s="18" t="s">
-        <v>9</v>
-      </c>
-      <c r="D22" s="7" t="s">
+      <c r="D23" s="18" t="s">
+        <v>9</v>
+      </c>
+      <c r="E23" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="E22" s="11"/>
-    </row>
-    <row r="23" spans="1:5" ht="15.75" thickBot="1">
-      <c r="A23" s="15">
+      <c r="F23" s="11"/>
+    </row>
+    <row r="24" spans="2:6" ht="15.75" thickBot="1">
+      <c r="B24" s="15">
         <v>22</v>
       </c>
-      <c r="B23" s="12">
+      <c r="C24" s="12">
         <v>1</v>
       </c>
-      <c r="C23" s="19" t="s">
-        <v>9</v>
-      </c>
-      <c r="D23" s="8" t="s">
+      <c r="D24" s="19" t="s">
+        <v>9</v>
+      </c>
+      <c r="E24" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="E23" s="12"/>
-    </row>
-    <row r="24" spans="1:5">
-      <c r="A24" s="13">
+      <c r="F24" s="12"/>
+    </row>
+    <row r="25" spans="2:6">
+      <c r="B25" s="13">
         <v>23</v>
       </c>
-      <c r="B24" s="10">
+      <c r="C25" s="10">
         <v>2</v>
       </c>
-      <c r="C24" s="17" t="s">
-        <v>9</v>
-      </c>
-      <c r="D24" s="6" t="s">
+      <c r="D25" s="17" t="s">
+        <v>9</v>
+      </c>
+      <c r="E25" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="E24" s="10"/>
-    </row>
-    <row r="25" spans="1:5">
-      <c r="A25" s="14">
+      <c r="F25" s="10"/>
+    </row>
+    <row r="26" spans="2:6">
+      <c r="B26" s="14">
         <v>24</v>
       </c>
-      <c r="B25" s="11">
+      <c r="C26" s="11">
         <v>3</v>
       </c>
-      <c r="C25" s="18" t="s">
-        <v>9</v>
-      </c>
-      <c r="D25" s="7" t="s">
+      <c r="D26" s="18" t="s">
+        <v>9</v>
+      </c>
+      <c r="E26" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="E25" s="11"/>
-    </row>
-    <row r="26" spans="1:5">
-      <c r="A26" s="14">
+      <c r="F26" s="11"/>
+    </row>
+    <row r="27" spans="2:6">
+      <c r="B27" s="14">
         <v>25</v>
       </c>
-      <c r="B26" s="11">
+      <c r="C27" s="11">
         <v>16</v>
       </c>
-      <c r="C26" s="18" t="s">
-        <v>9</v>
-      </c>
-      <c r="D26" s="7" t="s">
+      <c r="D27" s="18" t="s">
+        <v>9</v>
+      </c>
+      <c r="E27" s="7" t="s">
         <v>47</v>
       </c>
-      <c r="E26" s="11"/>
-    </row>
-    <row r="27" spans="1:5">
-      <c r="A27" s="14">
+      <c r="F27" s="11"/>
+    </row>
+    <row r="28" spans="2:6">
+      <c r="B28" s="14">
         <v>26</v>
       </c>
-      <c r="B27" s="11">
+      <c r="C28" s="11">
         <v>17</v>
       </c>
-      <c r="C27" s="18" t="s">
-        <v>9</v>
-      </c>
-      <c r="D27" s="7" t="s">
+      <c r="D28" s="18" t="s">
+        <v>9</v>
+      </c>
+      <c r="E28" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="E27" s="11"/>
-    </row>
-    <row r="28" spans="1:5">
-      <c r="A28" s="14">
+      <c r="F28" s="11"/>
+    </row>
+    <row r="29" spans="2:6">
+      <c r="B29" s="14">
         <v>27</v>
       </c>
-      <c r="B28" s="11" t="s">
-        <v>6</v>
-      </c>
-      <c r="C28" s="18" t="s">
-        <v>9</v>
-      </c>
-      <c r="D28" s="7" t="s">
+      <c r="C29" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="D29" s="18" t="s">
+        <v>9</v>
+      </c>
+      <c r="E29" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="E28" s="11"/>
-    </row>
-    <row r="29" spans="1:5">
-      <c r="A29" s="14">
+      <c r="F29" s="11"/>
+    </row>
+    <row r="30" spans="2:6">
+      <c r="B30" s="14">
         <v>28</v>
       </c>
-      <c r="B29" s="11" t="s">
-        <v>6</v>
-      </c>
-      <c r="C29" s="18" t="s">
-        <v>9</v>
-      </c>
-      <c r="D29" s="7" t="s">
+      <c r="C30" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="D30" s="18" t="s">
+        <v>9</v>
+      </c>
+      <c r="E30" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="E29" s="11"/>
-    </row>
-    <row r="30" spans="1:5">
-      <c r="A30" s="14">
+      <c r="F30" s="11"/>
+    </row>
+    <row r="31" spans="2:6">
+      <c r="B31" s="14">
         <v>29</v>
       </c>
-      <c r="B30" s="11" t="s">
-        <v>6</v>
-      </c>
-      <c r="C30" s="18" t="s">
-        <v>9</v>
-      </c>
-      <c r="D30" s="7" t="s">
+      <c r="C31" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="D31" s="18" t="s">
+        <v>9</v>
+      </c>
+      <c r="E31" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="E30" s="11"/>
-    </row>
-    <row r="31" spans="1:5">
-      <c r="A31" s="14">
+      <c r="F31" s="11"/>
+    </row>
+    <row r="32" spans="2:6">
+      <c r="B32" s="14">
         <v>30</v>
       </c>
-      <c r="B31" s="11" t="s">
-        <v>6</v>
-      </c>
-      <c r="C31" s="18" t="s">
-        <v>9</v>
-      </c>
-      <c r="D31" s="7" t="s">
+      <c r="C32" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="D32" s="18" t="s">
+        <v>9</v>
+      </c>
+      <c r="E32" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="E31" s="11"/>
-    </row>
-    <row r="32" spans="1:5">
-      <c r="A32" s="14">
+      <c r="F32" s="11"/>
+    </row>
+    <row r="33" spans="2:6">
+      <c r="B33" s="14">
         <v>31</v>
       </c>
-      <c r="B32" s="11" t="s">
-        <v>6</v>
-      </c>
-      <c r="C32" s="18" t="s">
-        <v>9</v>
-      </c>
-      <c r="D32" s="7" t="s">
+      <c r="C33" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="D33" s="18" t="s">
+        <v>9</v>
+      </c>
+      <c r="E33" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="E32" s="11"/>
-    </row>
-    <row r="33" spans="1:5">
-      <c r="A33" s="14">
+      <c r="F33" s="11"/>
+    </row>
+    <row r="34" spans="2:6">
+      <c r="B34" s="14">
         <v>32</v>
       </c>
-      <c r="B33" s="11" t="s">
-        <v>6</v>
-      </c>
-      <c r="C33" s="18" t="s">
-        <v>5</v>
-      </c>
-      <c r="D33" s="7" t="s">
+      <c r="C34" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="D34" s="18" t="s">
+        <v>5</v>
+      </c>
+      <c r="E34" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="E33" s="11"/>
-    </row>
-    <row r="34" spans="1:5" ht="15.75" thickBot="1">
-      <c r="A34" s="15">
+      <c r="F34" s="11"/>
+    </row>
+    <row r="35" spans="2:6" ht="15.75" thickBot="1">
+      <c r="B35" s="15">
         <v>33</v>
       </c>
-      <c r="B34" s="12">
+      <c r="C35" s="12">
         <v>4</v>
       </c>
-      <c r="C34" s="19" t="s">
-        <v>9</v>
-      </c>
-      <c r="D34" s="8" t="s">
+      <c r="D35" s="19" t="s">
+        <v>9</v>
+      </c>
+      <c r="E35" s="8" t="s">
         <v>34</v>
       </c>
-      <c r="E34" s="12"/>
-    </row>
-    <row r="35" spans="1:5">
-      <c r="A35" s="13">
+      <c r="F35" s="12"/>
+    </row>
+    <row r="36" spans="2:6">
+      <c r="B36" s="13">
         <v>34</v>
       </c>
-      <c r="B35" s="10" t="s">
-        <v>6</v>
-      </c>
-      <c r="C35" s="17" t="s">
-        <v>9</v>
-      </c>
-      <c r="D35" s="6" t="s">
+      <c r="C36" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="D36" s="17" t="s">
+        <v>9</v>
+      </c>
+      <c r="E36" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="E35" s="10"/>
-    </row>
-    <row r="36" spans="1:5">
-      <c r="A36" s="14">
+      <c r="F36" s="10"/>
+    </row>
+    <row r="37" spans="2:6">
+      <c r="B37" s="14">
         <v>35</v>
       </c>
-      <c r="B36" s="11" t="s">
-        <v>6</v>
-      </c>
-      <c r="C36" s="18" t="s">
-        <v>5</v>
-      </c>
-      <c r="D36" s="7" t="s">
+      <c r="C37" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="D37" s="18" t="s">
+        <v>5</v>
+      </c>
+      <c r="E37" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="E36" s="11"/>
-    </row>
-    <row r="37" spans="1:5">
-      <c r="A37" s="14">
+      <c r="F37" s="11"/>
+    </row>
+    <row r="38" spans="2:6">
+      <c r="B38" s="14">
         <v>36</v>
       </c>
-      <c r="B37" s="11">
+      <c r="C38" s="11">
         <v>19</v>
       </c>
-      <c r="C37" s="18" t="s">
-        <v>5</v>
-      </c>
-      <c r="D37" s="7" t="s">
+      <c r="D38" s="18" t="s">
+        <v>5</v>
+      </c>
+      <c r="E38" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="E37" s="11"/>
-    </row>
-    <row r="38" spans="1:5">
-      <c r="A38" s="14">
+      <c r="F38" s="11"/>
+    </row>
+    <row r="39" spans="2:6">
+      <c r="B39" s="14">
         <v>37</v>
       </c>
-      <c r="B38" s="11">
+      <c r="C39" s="11">
         <v>20</v>
       </c>
-      <c r="C38" s="18" t="s">
-        <v>5</v>
-      </c>
-      <c r="D38" s="7" t="s">
+      <c r="D39" s="18" t="s">
+        <v>5</v>
+      </c>
+      <c r="E39" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="E38" s="11"/>
-    </row>
-    <row r="39" spans="1:5">
-      <c r="A39" s="14">
+      <c r="F39" s="11"/>
+    </row>
+    <row r="40" spans="2:6">
+      <c r="B40" s="14">
         <v>38</v>
       </c>
-      <c r="B39" s="11">
+      <c r="C40" s="11">
         <v>21</v>
       </c>
-      <c r="C39" s="18" t="s">
-        <v>5</v>
-      </c>
-      <c r="D39" s="7" t="s">
+      <c r="D40" s="18" t="s">
+        <v>5</v>
+      </c>
+      <c r="E40" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="E39" s="11"/>
-    </row>
-    <row r="40" spans="1:5">
-      <c r="A40" s="14">
+      <c r="F40" s="11"/>
+    </row>
+    <row r="41" spans="2:6">
+      <c r="B41" s="14">
         <v>39</v>
       </c>
-      <c r="B40" s="11" t="s">
-        <v>6</v>
-      </c>
-      <c r="C40" s="18" t="s">
-        <v>9</v>
-      </c>
-      <c r="D40" s="7" t="s">
+      <c r="C41" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="D41" s="18" t="s">
+        <v>9</v>
+      </c>
+      <c r="E41" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="E40" s="11"/>
-    </row>
-    <row r="41" spans="1:5">
-      <c r="A41" s="14">
+      <c r="F41" s="11"/>
+    </row>
+    <row r="42" spans="2:6">
+      <c r="B42" s="14">
         <v>40</v>
       </c>
-      <c r="B41" s="11" t="s">
-        <v>6</v>
-      </c>
-      <c r="C41" s="18" t="s">
-        <v>9</v>
-      </c>
-      <c r="D41" s="7" t="s">
+      <c r="C42" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="D42" s="18" t="s">
+        <v>9</v>
+      </c>
+      <c r="E42" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="E41" s="11"/>
-    </row>
-    <row r="42" spans="1:5">
-      <c r="A42" s="14">
+      <c r="F42" s="11"/>
+    </row>
+    <row r="43" spans="2:6">
+      <c r="B43" s="14">
         <v>41</v>
       </c>
-      <c r="B42" s="11">
-        <v>5</v>
-      </c>
-      <c r="C42" s="18" t="s">
-        <v>5</v>
-      </c>
-      <c r="D42" s="7" t="s">
+      <c r="C43" s="11">
+        <v>5</v>
+      </c>
+      <c r="D43" s="18" t="s">
+        <v>5</v>
+      </c>
+      <c r="E43" s="7" t="s">
         <v>38</v>
       </c>
-      <c r="E42" s="11"/>
-    </row>
-    <row r="43" spans="1:5">
-      <c r="A43" s="14">
+      <c r="F43" s="11"/>
+    </row>
+    <row r="44" spans="2:6">
+      <c r="B44" s="14">
         <v>42</v>
       </c>
-      <c r="B43" s="11">
-        <v>6</v>
-      </c>
-      <c r="C43" s="18" t="s">
-        <v>5</v>
-      </c>
-      <c r="D43" s="7" t="s">
+      <c r="C44" s="11">
+        <v>6</v>
+      </c>
+      <c r="D44" s="18" t="s">
+        <v>5</v>
+      </c>
+      <c r="E44" s="7" t="s">
         <v>39</v>
       </c>
-      <c r="E43" s="11"/>
-    </row>
-    <row r="44" spans="1:5">
-      <c r="A44" s="14">
+      <c r="F44" s="11"/>
+    </row>
+    <row r="45" spans="2:6">
+      <c r="B45" s="14">
         <v>43</v>
       </c>
-      <c r="B44" s="11">
+      <c r="C45" s="11">
         <v>7</v>
       </c>
-      <c r="C44" s="18" t="s">
-        <v>5</v>
-      </c>
-      <c r="D44" s="7" t="s">
+      <c r="D45" s="18" t="s">
+        <v>5</v>
+      </c>
+      <c r="E45" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="E44" s="11"/>
-    </row>
-    <row r="45" spans="1:5" ht="15.75" thickBot="1">
-      <c r="A45" s="15">
+      <c r="F45" s="11"/>
+    </row>
+    <row r="46" spans="2:6" ht="15.75" thickBot="1">
+      <c r="B46" s="15">
         <v>44</v>
       </c>
-      <c r="B45" s="12">
+      <c r="C46" s="12">
         <v>8</v>
       </c>
-      <c r="C45" s="19" t="s">
-        <v>5</v>
-      </c>
-      <c r="D45" s="8" t="s">
+      <c r="D46" s="19" t="s">
+        <v>5</v>
+      </c>
+      <c r="E46" s="8" t="s">
         <v>41</v>
       </c>
-      <c r="E45" s="12"/>
+      <c r="F46" s="12"/>
     </row>
   </sheetData>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>